<commit_message>
proyecto y grafica excel
</commit_message>
<xml_diff>
--- a/03 - pandas/data/mi_df_colores.xlsx
+++ b/03 - pandas/data/mi_df_colores.xlsx
@@ -68,7 +68,7 @@
           <c:order val="0"/>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
@@ -82,10 +82,262 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Artistas!$B$2:$B$85</c:f>
+              <c:f>Sheet1!$B$2:$B$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="0"/>
+                <c:ptCount val="84"/>
+                <c:pt idx="0">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>

</xml_diff>